<commit_message>
New data from mazzo PC
</commit_message>
<xml_diff>
--- a/stats/statistics.xlsx
+++ b/stats/statistics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b09a39bcc1012fce/Documents/UniPr/magistrale/secondo_semestre/so_e_tempo_reale/programmi_sort/santa/stats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b09a39bcc1012fce/Documents/UniPr/magistrale/secondo_semestre/so_e_tempo_reale/programmi_sort/SantaClausProblem/stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{67ED1DCB-23F7-4196-AB18-5D8FACEDEB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3B3BFEF-FB8D-4B53-916C-C96E056A1D1D}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{67ED1DCB-23F7-4196-AB18-5D8FACEDEB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{651A0364-A290-47F9-86F2-09157BE6BEC2}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12216" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12216" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Delivery time" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Elves waiting time (2nd)" sheetId="4" r:id="rId4"/>
     <sheet name="Elves waiting time (3rd)" sheetId="5" r:id="rId5"/>
     <sheet name="Elves waiting time (4th)" sheetId="6" r:id="rId6"/>
+    <sheet name="Elves waiting time (5th)" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="24">
   <si>
     <t>santa_v1</t>
   </si>
@@ -254,6 +255,38 @@
       <t>) 4th</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>Elves waiting time in ms (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>santa_v3, list</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) 5th</t>
+    </r>
+  </si>
+  <si>
+    <t>Acer Nitro 5</t>
+  </si>
+  <si>
+    <t>ASUS TUF Gaming F15</t>
+  </si>
 </sst>
 </file>
 
@@ -389,7 +422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -455,12 +488,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
     <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="36">
     <dxf>
       <font>
         <b val="0"/>
@@ -597,6 +631,133 @@
           <bgColor rgb="FFFF6D6D"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2232,61 +2393,125 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>87711</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Immagine 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F23F3257-7BC5-85CE-88B5-CFF101F6AAC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="24479" t="22917" r="14062" b="11979"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6294120" y="982980"/>
+          <a:ext cx="6210300" cy="4934031"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18B675D9-1A46-4B9E-8A28-DDFCD9E39F51}" name="Tabella1" displayName="Tabella1" ref="B4:F52" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18B675D9-1A46-4B9E-8A28-DDFCD9E39F51}" name="Tabella1" displayName="Tabella1" ref="B4:F52" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="B4:F52" xr:uid="{18B675D9-1A46-4B9E-8A28-DDFCD9E39F51}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{68C9793C-3CE7-40C5-B12A-8900F1F2BC58}" name="#reindeer" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{02981B51-D820-4A61-8F87-5C973297C766}" name="#elves" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{BBBA96F3-B363-4150-A57C-F38AED59221F}" name="#santa" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{6F893902-C0F0-4313-A514-12FA6DFF381E}" name="Avergage" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{86D7F058-3DD3-4FED-B4FF-C7E1D0D0CEED}" name="Std.Dev." dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{68C9793C-3CE7-40C5-B12A-8900F1F2BC58}" name="#reindeer" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{02981B51-D820-4A61-8F87-5C973297C766}" name="#elves" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{BBBA96F3-B363-4150-A57C-F38AED59221F}" name="#santa" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{6F893902-C0F0-4313-A514-12FA6DFF381E}" name="Avergage" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{86D7F058-3DD3-4FED-B4FF-C7E1D0D0CEED}" name="Std.Dev." dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A39B2A33-B243-42A1-B8FE-DC2DD0CC89D6}" name="Tabella13" displayName="Tabella13" ref="B4:F52" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A39B2A33-B243-42A1-B8FE-DC2DD0CC89D6}" name="Tabella13" displayName="Tabella13" ref="B4:F52" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="B4:F52" xr:uid="{A39B2A33-B243-42A1-B8FE-DC2DD0CC89D6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D919451E-F7E6-4920-8AF3-89CB7875E493}" name="#reindeer" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{6173E1FA-D16C-4D56-9D2C-874660ECBECC}" name="#elves" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{69AF351C-DC2C-4E81-B786-EAA98C834955}" name="#santa" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{3D88D429-D733-4965-811A-0B0F4C5261A2}" name="Avergage" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{F1CE163C-D627-41C8-B06D-6834C35A9C2D}" name="Std.Dev." dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{D919451E-F7E6-4920-8AF3-89CB7875E493}" name="#reindeer" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{6173E1FA-D16C-4D56-9D2C-874660ECBECC}" name="#elves" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{69AF351C-DC2C-4E81-B786-EAA98C834955}" name="#santa" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{3D88D429-D733-4965-811A-0B0F4C5261A2}" name="Avergage" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{F1CE163C-D627-41C8-B06D-6834C35A9C2D}" name="Std.Dev." dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D62AA6BD-778C-4B8C-819D-731AAC815ED4}" name="Tabella134" displayName="Tabella134" ref="B4:F52" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D62AA6BD-778C-4B8C-819D-731AAC815ED4}" name="Tabella134" displayName="Tabella134" ref="B4:F52" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="B4:F52" xr:uid="{D62AA6BD-778C-4B8C-819D-731AAC815ED4}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{57B6EDB4-68BC-452C-A1CC-F02DF4D8D251}" name="#reindeer" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{D203EB9D-013C-4F7C-A372-3FB7CB2A5888}" name="#elves" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{52061BDA-34A7-470C-AA2F-8E68C8608C63}" name="#santa" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{3BB9B3CE-8B9C-48BE-B38A-1C73C2521F7E}" name="Avergage" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{BCC6D40D-FE2C-4585-B668-27AEEC8E9FD5}" name="Std.Dev." dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{57B6EDB4-68BC-452C-A1CC-F02DF4D8D251}" name="#reindeer" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{D203EB9D-013C-4F7C-A372-3FB7CB2A5888}" name="#elves" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{52061BDA-34A7-470C-AA2F-8E68C8608C63}" name="#santa" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{3BB9B3CE-8B9C-48BE-B38A-1C73C2521F7E}" name="Avergage" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{BCC6D40D-FE2C-4585-B668-27AEEC8E9FD5}" name="Std.Dev." dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{845B5C2A-09D4-4A3A-B84E-D1FFE2298ED8}" name="Tabella1345" displayName="Tabella1345" ref="B4:F52" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{845B5C2A-09D4-4A3A-B84E-D1FFE2298ED8}" name="Tabella1345" displayName="Tabella1345" ref="B4:F52" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="B4:F52" xr:uid="{845B5C2A-09D4-4A3A-B84E-D1FFE2298ED8}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7B943B3A-9A89-4F9F-A853-5A9814D469E3}" name="#reindeer" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{A6EEF20A-E28C-4A48-8956-795333ACE39D}" name="#elves" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{457D674E-6A2D-4CDE-95DA-23BE2DB06917}" name="#santa" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{75A64399-1220-4A29-BF03-DE8A45A38951}" name="Avergage" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{8BAF1286-C858-4EFA-A585-F7D1D33611FD}" name="Std.Dev." dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{7B943B3A-9A89-4F9F-A853-5A9814D469E3}" name="#reindeer" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{A6EEF20A-E28C-4A48-8956-795333ACE39D}" name="#elves" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{457D674E-6A2D-4CDE-95DA-23BE2DB06917}" name="#santa" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{75A64399-1220-4A29-BF03-DE8A45A38951}" name="Avergage" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{8BAF1286-C858-4EFA-A585-F7D1D33611FD}" name="Std.Dev." dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{20891BED-2C54-4B17-8266-CBD2F440FEE9}" name="Tabella13456" displayName="Tabella13456" ref="B4:F52" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="B4:F52" xr:uid="{20891BED-2C54-4B17-8266-CBD2F440FEE9}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{9053EC05-B09C-4709-B01A-ACB4CA07722D}" name="#reindeer" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{684A9087-046B-4660-9A40-98D629C59C5F}" name="#elves" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{6E77BF1C-799D-4BE6-B78C-5CA49D1F7BB6}" name="#santa" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{E5670B8F-6E79-4951-A7AA-3021EE6AB1D9}" name="Avergage" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{47117608-6242-4D43-A6C6-C57C9DE4C2B0}" name="Std.Dev." dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11620,7 +11845,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -11639,6 +11864,11 @@
         <v>17</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
         <v>13</v>
@@ -12474,9 +12704,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -12486,7 +12717,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -12505,6 +12736,11 @@
         <v>18</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
         <v>13</v>
@@ -13352,7 +13588,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -13371,6 +13607,11 @@
         <v>19</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
         <v>13</v>
@@ -14215,6 +14456,878 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4BC096-8A3D-4DAD-A146-92F5CE6C6C59}">
+  <dimension ref="A1:F52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="18"/>
+    <col min="2" max="2" width="14.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="18">
+        <v>9</v>
+      </c>
+      <c r="C5" s="18">
+        <v>3</v>
+      </c>
+      <c r="D5" s="18">
+        <v>1</v>
+      </c>
+      <c r="E5" s="18">
+        <v>2.3920089999999998</v>
+      </c>
+      <c r="F5" s="18">
+        <v>38.350158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="18">
+        <v>9</v>
+      </c>
+      <c r="C6" s="18">
+        <v>3</v>
+      </c>
+      <c r="D6" s="18">
+        <v>2</v>
+      </c>
+      <c r="E6" s="18">
+        <v>3.3172100000000002</v>
+      </c>
+      <c r="F6" s="18">
+        <v>21.847456000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="18">
+        <v>9</v>
+      </c>
+      <c r="C7" s="18">
+        <v>4</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1</v>
+      </c>
+      <c r="E7" s="18">
+        <v>1.5612349999999999</v>
+      </c>
+      <c r="F7" s="18">
+        <v>1.473503</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="18">
+        <v>9</v>
+      </c>
+      <c r="C8" s="18">
+        <v>4</v>
+      </c>
+      <c r="D8" s="18">
+        <v>2</v>
+      </c>
+      <c r="E8" s="18">
+        <v>6.7072669999999999</v>
+      </c>
+      <c r="F8" s="18">
+        <v>25.510134999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="18">
+        <v>9</v>
+      </c>
+      <c r="C9" s="18">
+        <v>5</v>
+      </c>
+      <c r="D9" s="18">
+        <v>1</v>
+      </c>
+      <c r="E9" s="18">
+        <v>1.616854</v>
+      </c>
+      <c r="F9" s="18">
+        <v>1.3446149999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="18">
+        <v>9</v>
+      </c>
+      <c r="C10" s="18">
+        <v>5</v>
+      </c>
+      <c r="D10" s="18">
+        <v>2</v>
+      </c>
+      <c r="E10" s="18">
+        <v>9.9307619999999996</v>
+      </c>
+      <c r="F10" s="18">
+        <v>24.693231999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="18">
+        <v>9</v>
+      </c>
+      <c r="C11" s="18">
+        <v>6</v>
+      </c>
+      <c r="D11" s="18">
+        <v>1</v>
+      </c>
+      <c r="E11" s="18">
+        <v>2.5645340000000001</v>
+      </c>
+      <c r="F11" s="18">
+        <v>45.55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="18">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18">
+        <v>6</v>
+      </c>
+      <c r="D12" s="18">
+        <v>2</v>
+      </c>
+      <c r="E12" s="18">
+        <v>13.407348000000001</v>
+      </c>
+      <c r="F12" s="18">
+        <v>32.253472000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="18">
+        <v>9</v>
+      </c>
+      <c r="C13" s="18">
+        <v>6</v>
+      </c>
+      <c r="D13" s="18">
+        <v>3</v>
+      </c>
+      <c r="E13" s="18">
+        <v>2.307118</v>
+      </c>
+      <c r="F13" s="18">
+        <v>13.711421</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="18">
+        <v>9</v>
+      </c>
+      <c r="C14" s="18">
+        <v>7</v>
+      </c>
+      <c r="D14" s="18">
+        <v>1</v>
+      </c>
+      <c r="E14" s="18">
+        <v>1.33206</v>
+      </c>
+      <c r="F14" s="18">
+        <v>2.0443899999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="18">
+        <v>9</v>
+      </c>
+      <c r="C15" s="18">
+        <v>7</v>
+      </c>
+      <c r="D15" s="18">
+        <v>2</v>
+      </c>
+      <c r="E15" s="18">
+        <v>16.845123000000001</v>
+      </c>
+      <c r="F15" s="18">
+        <v>33.017499000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="18">
+        <v>9</v>
+      </c>
+      <c r="C16" s="18">
+        <v>7</v>
+      </c>
+      <c r="D16" s="18">
+        <v>3</v>
+      </c>
+      <c r="E16" s="18">
+        <v>4.3136599999999996</v>
+      </c>
+      <c r="F16" s="18">
+        <v>15.053824000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="18">
+        <v>9</v>
+      </c>
+      <c r="C17" s="18">
+        <v>8</v>
+      </c>
+      <c r="D17" s="18">
+        <v>1</v>
+      </c>
+      <c r="E17" s="18">
+        <v>1.166399</v>
+      </c>
+      <c r="F17" s="18">
+        <v>1.246156</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="18">
+        <v>9</v>
+      </c>
+      <c r="C18" s="18">
+        <v>8</v>
+      </c>
+      <c r="D18" s="18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="18">
+        <v>20.048573999999999</v>
+      </c>
+      <c r="F18" s="18">
+        <v>34.046677000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="18">
+        <v>9</v>
+      </c>
+      <c r="C19" s="18">
+        <v>8</v>
+      </c>
+      <c r="D19" s="18">
+        <v>3</v>
+      </c>
+      <c r="E19" s="18">
+        <v>7.0839119999999998</v>
+      </c>
+      <c r="F19" s="18">
+        <v>19.645251999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="18">
+        <v>9</v>
+      </c>
+      <c r="C20" s="18">
+        <v>9</v>
+      </c>
+      <c r="D20" s="18">
+        <v>1</v>
+      </c>
+      <c r="E20" s="18">
+        <v>1.219508</v>
+      </c>
+      <c r="F20" s="18">
+        <v>1.42808</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="18">
+        <v>9</v>
+      </c>
+      <c r="C21" s="18">
+        <v>9</v>
+      </c>
+      <c r="D21" s="18">
+        <v>2</v>
+      </c>
+      <c r="E21" s="18">
+        <v>24.366001000000001</v>
+      </c>
+      <c r="F21" s="18">
+        <v>40.514758</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="18">
+        <v>9</v>
+      </c>
+      <c r="C22" s="18">
+        <v>9</v>
+      </c>
+      <c r="D22" s="18">
+        <v>3</v>
+      </c>
+      <c r="E22" s="18">
+        <v>7.8384600000000004</v>
+      </c>
+      <c r="F22" s="18">
+        <v>16.145669999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="18">
+        <v>9</v>
+      </c>
+      <c r="C23" s="18">
+        <v>9</v>
+      </c>
+      <c r="D23" s="18">
+        <v>4</v>
+      </c>
+      <c r="E23" s="18">
+        <v>2.933916</v>
+      </c>
+      <c r="F23" s="18">
+        <v>13.859855</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="18">
+        <v>9</v>
+      </c>
+      <c r="C24" s="18">
+        <v>10</v>
+      </c>
+      <c r="D24" s="18">
+        <v>1</v>
+      </c>
+      <c r="E24" s="18">
+        <v>1.199424</v>
+      </c>
+      <c r="F24" s="18">
+        <v>1.164339</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="18">
+        <v>9</v>
+      </c>
+      <c r="C25" s="18">
+        <v>10</v>
+      </c>
+      <c r="D25" s="18">
+        <v>2</v>
+      </c>
+      <c r="E25" s="18">
+        <v>26.991503000000002</v>
+      </c>
+      <c r="F25" s="18">
+        <v>40.378539000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="18">
+        <v>9</v>
+      </c>
+      <c r="C26" s="18">
+        <v>10</v>
+      </c>
+      <c r="D26" s="18">
+        <v>3</v>
+      </c>
+      <c r="E26" s="18">
+        <v>10.662815999999999</v>
+      </c>
+      <c r="F26" s="18">
+        <v>21.027450999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="18">
+        <v>9</v>
+      </c>
+      <c r="C27" s="18">
+        <v>10</v>
+      </c>
+      <c r="D27" s="18">
+        <v>4</v>
+      </c>
+      <c r="E27" s="18">
+        <v>3.828217</v>
+      </c>
+      <c r="F27" s="18">
+        <v>16.672011000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="18">
+        <v>9</v>
+      </c>
+      <c r="C28" s="18">
+        <v>11</v>
+      </c>
+      <c r="D28" s="18">
+        <v>1</v>
+      </c>
+      <c r="E28" s="18">
+        <v>1.822173</v>
+      </c>
+      <c r="F28" s="18">
+        <v>48.790897999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="18">
+        <v>9</v>
+      </c>
+      <c r="C29" s="18">
+        <v>11</v>
+      </c>
+      <c r="D29" s="18">
+        <v>2</v>
+      </c>
+      <c r="E29" s="18">
+        <v>30.665904999999999</v>
+      </c>
+      <c r="F29" s="18">
+        <v>45.051082999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="18">
+        <v>9</v>
+      </c>
+      <c r="C30" s="18">
+        <v>11</v>
+      </c>
+      <c r="D30" s="18">
+        <v>3</v>
+      </c>
+      <c r="E30" s="18">
+        <v>12.27136</v>
+      </c>
+      <c r="F30" s="18">
+        <v>23.063123000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="18">
+        <v>9</v>
+      </c>
+      <c r="C31" s="18">
+        <v>11</v>
+      </c>
+      <c r="D31" s="18">
+        <v>4</v>
+      </c>
+      <c r="E31" s="18">
+        <v>5.568816</v>
+      </c>
+      <c r="F31" s="18">
+        <v>15.446676999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="18">
+        <v>9</v>
+      </c>
+      <c r="C32" s="18">
+        <v>12</v>
+      </c>
+      <c r="D32" s="18">
+        <v>1</v>
+      </c>
+      <c r="E32" s="18">
+        <v>0.98755199999999999</v>
+      </c>
+      <c r="F32" s="18">
+        <v>0.95560500000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="18">
+        <v>9</v>
+      </c>
+      <c r="C33" s="18">
+        <v>12</v>
+      </c>
+      <c r="D33" s="18">
+        <v>2</v>
+      </c>
+      <c r="E33" s="18">
+        <v>33.979979999999998</v>
+      </c>
+      <c r="F33" s="18">
+        <v>46.035863999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="18">
+        <v>9</v>
+      </c>
+      <c r="C34" s="18">
+        <v>12</v>
+      </c>
+      <c r="D34" s="18">
+        <v>3</v>
+      </c>
+      <c r="E34" s="18">
+        <v>13.558973999999999</v>
+      </c>
+      <c r="F34" s="18">
+        <v>21.371752999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="18">
+        <v>9</v>
+      </c>
+      <c r="C35" s="18">
+        <v>12</v>
+      </c>
+      <c r="D35" s="18">
+        <v>4</v>
+      </c>
+      <c r="E35" s="18">
+        <v>7.0352209999999999</v>
+      </c>
+      <c r="F35" s="18">
+        <v>14.899762000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="18">
+        <v>9</v>
+      </c>
+      <c r="C36" s="18">
+        <v>12</v>
+      </c>
+      <c r="D36" s="18">
+        <v>5</v>
+      </c>
+      <c r="E36" s="18">
+        <v>3.2497549999999999</v>
+      </c>
+      <c r="F36" s="18">
+        <v>13.196353999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="18">
+        <v>9</v>
+      </c>
+      <c r="C37" s="18">
+        <v>13</v>
+      </c>
+      <c r="D37" s="18">
+        <v>1</v>
+      </c>
+      <c r="E37" s="18">
+        <v>1.0749200000000001</v>
+      </c>
+      <c r="F37" s="18">
+        <v>0.648231</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="18">
+        <v>9</v>
+      </c>
+      <c r="C38" s="18">
+        <v>13</v>
+      </c>
+      <c r="D38" s="18">
+        <v>2</v>
+      </c>
+      <c r="E38" s="18">
+        <v>38.143062</v>
+      </c>
+      <c r="F38" s="18">
+        <v>51.419215999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="18">
+        <v>9</v>
+      </c>
+      <c r="C39" s="18">
+        <v>13</v>
+      </c>
+      <c r="D39" s="18">
+        <v>3</v>
+      </c>
+      <c r="E39" s="18">
+        <v>16.845321999999999</v>
+      </c>
+      <c r="F39" s="18">
+        <v>41.206721999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="18">
+        <v>9</v>
+      </c>
+      <c r="C40" s="18">
+        <v>13</v>
+      </c>
+      <c r="D40" s="18">
+        <v>4</v>
+      </c>
+      <c r="E40" s="18">
+        <v>8.8782270000000008</v>
+      </c>
+      <c r="F40" s="18">
+        <v>20.003125000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="18">
+        <v>9</v>
+      </c>
+      <c r="C41" s="18">
+        <v>13</v>
+      </c>
+      <c r="D41" s="18">
+        <v>5</v>
+      </c>
+      <c r="E41" s="18">
+        <v>4.3377559999999997</v>
+      </c>
+      <c r="F41" s="18">
+        <v>13.820251000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="18">
+        <v>9</v>
+      </c>
+      <c r="C42" s="18">
+        <v>14</v>
+      </c>
+      <c r="D42" s="18">
+        <v>1</v>
+      </c>
+      <c r="E42" s="18">
+        <v>1.2430429999999999</v>
+      </c>
+      <c r="F42" s="18">
+        <v>3.0217480000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="18">
+        <v>9</v>
+      </c>
+      <c r="C43" s="18">
+        <v>14</v>
+      </c>
+      <c r="D43" s="18">
+        <v>2</v>
+      </c>
+      <c r="E43" s="18">
+        <v>41.738278999999999</v>
+      </c>
+      <c r="F43" s="18">
+        <v>53.700141000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="18">
+        <v>9</v>
+      </c>
+      <c r="C44" s="18">
+        <v>14</v>
+      </c>
+      <c r="D44" s="18">
+        <v>3</v>
+      </c>
+      <c r="E44" s="18">
+        <v>18.741313000000002</v>
+      </c>
+      <c r="F44" s="18">
+        <v>29.899104999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="18">
+        <v>9</v>
+      </c>
+      <c r="C45" s="18">
+        <v>14</v>
+      </c>
+      <c r="D45" s="18">
+        <v>4</v>
+      </c>
+      <c r="E45" s="18">
+        <v>10.130501000000001</v>
+      </c>
+      <c r="F45" s="18">
+        <v>20.352793999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="18">
+        <v>9</v>
+      </c>
+      <c r="C46" s="18">
+        <v>14</v>
+      </c>
+      <c r="D46" s="18">
+        <v>5</v>
+      </c>
+      <c r="E46" s="18">
+        <v>5.6467640000000001</v>
+      </c>
+      <c r="F46" s="18">
+        <v>15.576309999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="18">
+        <v>9</v>
+      </c>
+      <c r="C47" s="18">
+        <v>15</v>
+      </c>
+      <c r="D47" s="18">
+        <v>1</v>
+      </c>
+      <c r="E47" s="18">
+        <v>1.0843469999999999</v>
+      </c>
+      <c r="F47" s="18">
+        <v>0.61018399999999995</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="18">
+        <v>9</v>
+      </c>
+      <c r="C48" s="18">
+        <v>15</v>
+      </c>
+      <c r="D48" s="18">
+        <v>2</v>
+      </c>
+      <c r="E48" s="18">
+        <v>44.391537999999997</v>
+      </c>
+      <c r="F48" s="18">
+        <v>54.021039000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="18">
+        <v>9</v>
+      </c>
+      <c r="C49" s="18">
+        <v>15</v>
+      </c>
+      <c r="D49" s="18">
+        <v>3</v>
+      </c>
+      <c r="E49" s="18">
+        <v>20.646245</v>
+      </c>
+      <c r="F49" s="18">
+        <v>30.121179999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="18">
+        <v>9</v>
+      </c>
+      <c r="C50" s="18">
+        <v>15</v>
+      </c>
+      <c r="D50" s="18">
+        <v>4</v>
+      </c>
+      <c r="E50" s="18">
+        <v>12.088473</v>
+      </c>
+      <c r="F50" s="18">
+        <v>21.944828000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="18">
+        <v>9</v>
+      </c>
+      <c r="C51" s="18">
+        <v>15</v>
+      </c>
+      <c r="D51" s="18">
+        <v>5</v>
+      </c>
+      <c r="E51" s="18">
+        <v>6.8606860000000003</v>
+      </c>
+      <c r="F51" s="18">
+        <v>19.432787000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="18">
+        <v>9</v>
+      </c>
+      <c r="C52" s="18">
+        <v>15</v>
+      </c>
+      <c r="D52" s="18">
+        <v>6</v>
+      </c>
+      <c r="E52" s="18">
+        <v>3.9206780000000001</v>
+      </c>
+      <c r="F52" s="18">
+        <v>14.173537</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5958168B-79F8-46C8-969C-A8B0B51C678F}">
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -14232,7 +15345,12 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -14263,10 +15381,10 @@
         <v>1</v>
       </c>
       <c r="E5" s="18">
-        <v>2.3920089999999998</v>
+        <v>26.551203999999998</v>
       </c>
       <c r="F5" s="18">
-        <v>38.350158</v>
+        <v>207.20390399999999</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -14280,10 +15398,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="18">
-        <v>3.3172100000000002</v>
+        <v>2.033061</v>
       </c>
       <c r="F6" s="18">
-        <v>21.847456000000001</v>
+        <v>13.449821999999999</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -14297,10 +15415,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="18">
-        <v>1.5612349999999999</v>
+        <v>30.537348999999999</v>
       </c>
       <c r="F7" s="18">
-        <v>1.473503</v>
+        <v>245.98041599999999</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -14314,10 +15432,10 @@
         <v>2</v>
       </c>
       <c r="E8" s="18">
-        <v>6.7072669999999999</v>
+        <v>5.4427830000000004</v>
       </c>
       <c r="F8" s="18">
-        <v>25.510134999999998</v>
+        <v>21.720683999999999</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -14331,10 +15449,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="18">
-        <v>1.616854</v>
+        <v>19.630436</v>
       </c>
       <c r="F9" s="18">
-        <v>1.3446149999999999</v>
+        <v>217.67732899999999</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -14348,10 +15466,10 @@
         <v>2</v>
       </c>
       <c r="E10" s="18">
-        <v>9.9307619999999996</v>
+        <v>7.7984210000000003</v>
       </c>
       <c r="F10" s="18">
-        <v>24.693231999999998</v>
+        <v>18.281195</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -14365,10 +15483,10 @@
         <v>1</v>
       </c>
       <c r="E11" s="18">
-        <v>2.5645340000000001</v>
+        <v>23.460813999999999</v>
       </c>
       <c r="F11" s="18">
-        <v>45.55</v>
+        <v>258.09037799999999</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -14382,10 +15500,10 @@
         <v>2</v>
       </c>
       <c r="E12" s="18">
-        <v>13.407348000000001</v>
+        <v>11.393704</v>
       </c>
       <c r="F12" s="18">
-        <v>32.253472000000002</v>
+        <v>22.824207999999999</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -14399,10 +15517,10 @@
         <v>3</v>
       </c>
       <c r="E13" s="18">
-        <v>2.307118</v>
+        <v>1.137343</v>
       </c>
       <c r="F13" s="18">
-        <v>13.711421</v>
+        <v>7.922536</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -14416,10 +15534,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="18">
-        <v>1.33206</v>
+        <v>11.654083</v>
       </c>
       <c r="F14" s="18">
-        <v>2.0443899999999999</v>
+        <v>174.54871800000001</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -14433,10 +15551,10 @@
         <v>2</v>
       </c>
       <c r="E15" s="18">
-        <v>16.845123000000001</v>
+        <v>14.990512000000001</v>
       </c>
       <c r="F15" s="18">
-        <v>33.017499000000001</v>
+        <v>30.80564</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -14450,10 +15568,10 @@
         <v>3</v>
       </c>
       <c r="E16" s="18">
-        <v>4.3136599999999996</v>
+        <v>2.6891120000000002</v>
       </c>
       <c r="F16" s="18">
-        <v>15.053824000000001</v>
+        <v>8.7042730000000006</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -14467,10 +15585,10 @@
         <v>1</v>
       </c>
       <c r="E17" s="18">
-        <v>1.166399</v>
+        <v>12.683559000000001</v>
       </c>
       <c r="F17" s="18">
-        <v>1.246156</v>
+        <v>185.838684</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -14484,10 +15602,10 @@
         <v>2</v>
       </c>
       <c r="E18" s="18">
-        <v>20.048573999999999</v>
+        <v>17.382783</v>
       </c>
       <c r="F18" s="18">
-        <v>34.046677000000003</v>
+        <v>25.882346999999999</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -14501,10 +15619,10 @@
         <v>3</v>
       </c>
       <c r="E19" s="18">
-        <v>7.0839119999999998</v>
+        <v>4.4186880000000004</v>
       </c>
       <c r="F19" s="18">
-        <v>19.645251999999999</v>
+        <v>8.7374500000000008</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -14518,10 +15636,10 @@
         <v>1</v>
       </c>
       <c r="E20" s="18">
-        <v>1.219508</v>
+        <v>13.503379000000001</v>
       </c>
       <c r="F20" s="18">
-        <v>1.42808</v>
+        <v>192.77699899999999</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -14535,10 +15653,10 @@
         <v>2</v>
       </c>
       <c r="E21" s="18">
-        <v>24.366001000000001</v>
+        <v>20.258986</v>
       </c>
       <c r="F21" s="18">
-        <v>40.514758</v>
+        <v>28.836863000000001</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -14552,10 +15670,10 @@
         <v>3</v>
       </c>
       <c r="E22" s="18">
-        <v>7.8384600000000004</v>
+        <v>6.2580280000000004</v>
       </c>
       <c r="F22" s="18">
-        <v>16.145669999999999</v>
+        <v>10.673487</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -14569,10 +15687,10 @@
         <v>4</v>
       </c>
       <c r="E23" s="18">
-        <v>2.933916</v>
+        <v>0.94094599999999995</v>
       </c>
       <c r="F23" s="18">
-        <v>13.859855</v>
+        <v>7.9345189999999999</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -14586,10 +15704,10 @@
         <v>1</v>
       </c>
       <c r="E24" s="18">
-        <v>1.199424</v>
+        <v>26.662348999999999</v>
       </c>
       <c r="F24" s="18">
-        <v>1.164339</v>
+        <v>270.22112499999997</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -14603,10 +15721,10 @@
         <v>2</v>
       </c>
       <c r="E25" s="18">
-        <v>26.991503000000002</v>
+        <v>25.009160999999999</v>
       </c>
       <c r="F25" s="18">
-        <v>40.378539000000004</v>
+        <v>36.811304</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -14620,10 +15738,10 @@
         <v>3</v>
       </c>
       <c r="E26" s="18">
-        <v>10.662815999999999</v>
+        <v>8.30335</v>
       </c>
       <c r="F26" s="18">
-        <v>21.027450999999999</v>
+        <v>14.477100999999999</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -14637,10 +15755,10 @@
         <v>4</v>
       </c>
       <c r="E27" s="18">
-        <v>3.828217</v>
+        <v>2.273285</v>
       </c>
       <c r="F27" s="18">
-        <v>16.672011000000001</v>
+        <v>7.3157490000000003</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -14654,10 +15772,10 @@
         <v>1</v>
       </c>
       <c r="E28" s="18">
-        <v>1.822173</v>
+        <v>51.325825999999999</v>
       </c>
       <c r="F28" s="18">
-        <v>48.790897999999999</v>
+        <v>388.13014399999997</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -14671,10 +15789,10 @@
         <v>2</v>
       </c>
       <c r="E29" s="18">
-        <v>30.665904999999999</v>
+        <v>26.048445000000001</v>
       </c>
       <c r="F29" s="18">
-        <v>45.051082999999998</v>
+        <v>33.838580999999998</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -14688,10 +15806,10 @@
         <v>3</v>
       </c>
       <c r="E30" s="18">
-        <v>12.27136</v>
+        <v>9.6326630000000009</v>
       </c>
       <c r="F30" s="18">
-        <v>23.063123000000001</v>
+        <v>13.108397999999999</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
@@ -14705,10 +15823,10 @@
         <v>4</v>
       </c>
       <c r="E31" s="18">
-        <v>5.568816</v>
+        <v>3.3668719999999999</v>
       </c>
       <c r="F31" s="18">
-        <v>15.446676999999999</v>
+        <v>9.0832689999999996</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -14722,10 +15840,10 @@
         <v>1</v>
       </c>
       <c r="E32" s="18">
-        <v>0.98755199999999999</v>
+        <v>49.897151000000001</v>
       </c>
       <c r="F32" s="18">
-        <v>0.95560500000000004</v>
+        <v>385.76495399999999</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
@@ -14739,10 +15857,10 @@
         <v>2</v>
       </c>
       <c r="E33" s="18">
-        <v>33.979979999999998</v>
+        <v>30.172416999999999</v>
       </c>
       <c r="F33" s="18">
-        <v>46.035863999999997</v>
+        <v>35.797835999999997</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -14756,10 +15874,10 @@
         <v>3</v>
       </c>
       <c r="E34" s="18">
-        <v>13.558973999999999</v>
+        <v>12.256379000000001</v>
       </c>
       <c r="F34" s="18">
-        <v>21.371752999999998</v>
+        <v>15.290703000000001</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -14773,10 +15891,10 @@
         <v>4</v>
       </c>
       <c r="E35" s="18">
-        <v>7.0352209999999999</v>
+        <v>4.9505379999999999</v>
       </c>
       <c r="F35" s="18">
-        <v>14.899762000000001</v>
+        <v>11.638636</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -14790,10 +15908,10 @@
         <v>5</v>
       </c>
       <c r="E36" s="18">
-        <v>3.2497549999999999</v>
+        <v>1.440661</v>
       </c>
       <c r="F36" s="18">
-        <v>13.196353999999999</v>
+        <v>13.126606000000001</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -14807,10 +15925,10 @@
         <v>1</v>
       </c>
       <c r="E37" s="18">
-        <v>1.0749200000000001</v>
+        <v>52.144897</v>
       </c>
       <c r="F37" s="18">
-        <v>0.648231</v>
+        <v>390.41503899999998</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -14824,10 +15942,10 @@
         <v>2</v>
       </c>
       <c r="E38" s="18">
-        <v>38.143062</v>
+        <v>33.917833999999999</v>
       </c>
       <c r="F38" s="18">
-        <v>51.419215999999999</v>
+        <v>41.306126999999996</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -14841,10 +15959,10 @@
         <v>3</v>
       </c>
       <c r="E39" s="18">
-        <v>16.845321999999999</v>
+        <v>13.677391</v>
       </c>
       <c r="F39" s="18">
-        <v>41.206721999999999</v>
+        <v>15.712368</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -14858,10 +15976,10 @@
         <v>4</v>
       </c>
       <c r="E40" s="18">
-        <v>8.8782270000000008</v>
+        <v>6.2771600000000003</v>
       </c>
       <c r="F40" s="18">
-        <v>20.003125000000001</v>
+        <v>11.018959000000001</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
@@ -14875,10 +15993,10 @@
         <v>5</v>
       </c>
       <c r="E41" s="18">
-        <v>4.3377559999999997</v>
+        <v>1.925116</v>
       </c>
       <c r="F41" s="18">
-        <v>13.820251000000001</v>
+        <v>3.4798420000000001</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
@@ -14892,10 +16010,10 @@
         <v>1</v>
       </c>
       <c r="E42" s="18">
-        <v>1.2430429999999999</v>
+        <v>44.096142</v>
       </c>
       <c r="F42" s="18">
-        <v>3.0217480000000001</v>
+        <v>365.90262999999999</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
@@ -14909,10 +16027,10 @@
         <v>2</v>
       </c>
       <c r="E43" s="18">
-        <v>41.738278999999999</v>
+        <v>36.558908000000002</v>
       </c>
       <c r="F43" s="18">
-        <v>53.700141000000002</v>
+        <v>41.570000999999998</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
@@ -14926,10 +16044,10 @@
         <v>3</v>
       </c>
       <c r="E44" s="18">
-        <v>18.741313000000002</v>
+        <v>15.271572000000001</v>
       </c>
       <c r="F44" s="18">
-        <v>29.899104999999999</v>
+        <v>16.284020000000002</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
@@ -14943,10 +16061,10 @@
         <v>4</v>
       </c>
       <c r="E45" s="18">
-        <v>10.130501000000001</v>
+        <v>7.1809450000000004</v>
       </c>
       <c r="F45" s="18">
-        <v>20.352793999999999</v>
+        <v>8.1305429999999994</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
@@ -14960,10 +16078,10 @@
         <v>5</v>
       </c>
       <c r="E46" s="18">
-        <v>5.6467640000000001</v>
+        <v>2.9775659999999999</v>
       </c>
       <c r="F46" s="18">
-        <v>15.576309999999999</v>
+        <v>5.3430220000000004</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
@@ -14977,10 +16095,10 @@
         <v>1</v>
       </c>
       <c r="E47" s="18">
-        <v>1.0843469999999999</v>
+        <v>46.631154000000002</v>
       </c>
       <c r="F47" s="18">
-        <v>0.61018399999999995</v>
+        <v>378.89781599999998</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
@@ -14994,10 +16112,10 @@
         <v>2</v>
       </c>
       <c r="E48" s="18">
-        <v>44.391537999999997</v>
+        <v>39.891852</v>
       </c>
       <c r="F48" s="18">
-        <v>54.021039000000002</v>
+        <v>43.090541000000002</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
@@ -15011,10 +16129,10 @@
         <v>3</v>
       </c>
       <c r="E49" s="18">
-        <v>20.646245</v>
+        <v>16.040735999999999</v>
       </c>
       <c r="F49" s="18">
-        <v>30.121179999999999</v>
+        <v>20.354051999999999</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
@@ -15028,10 +16146,10 @@
         <v>4</v>
       </c>
       <c r="E50" s="18">
-        <v>12.088473</v>
+        <v>7.6564180000000004</v>
       </c>
       <c r="F50" s="18">
-        <v>21.944828000000001</v>
+        <v>8.3987180000000006</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
@@ -15045,10 +16163,10 @@
         <v>5</v>
       </c>
       <c r="E51" s="18">
-        <v>6.8606860000000003</v>
+        <v>3.566395</v>
       </c>
       <c r="F51" s="18">
-        <v>19.432787000000001</v>
+        <v>13.141807</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
@@ -15062,10 +16180,10 @@
         <v>6</v>
       </c>
       <c r="E52" s="18">
-        <v>3.9206780000000001</v>
+        <v>0.74803799999999998</v>
       </c>
       <c r="F52" s="18">
-        <v>14.173537</v>
+        <v>6.0638680000000003</v>
       </c>
     </row>
   </sheetData>
@@ -15079,15 +16197,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101005E88FE40BA4E0D4EA2BBF58D03FB6876" ma:contentTypeVersion="14" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="e417158f90a3e000520a4c3f7a238cdd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e6c0028f-6bbf-472a-b529-33761164d13b" xmlns:ns3="8c489475-599a-4bcd-8c75-be2b892c5853" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c1a052372813eabbbab35c07dbce5fa2" ns2:_="" ns3:_="">
     <xsd:import namespace="e6c0028f-6bbf-472a-b529-33761164d13b"/>
@@ -15316,15 +16425,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43BAA3F7-B280-41FD-9E33-AA955AC1A934}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64F7475F-68A6-4CE5-89DE-205D63BB1E24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15341,4 +16451,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43BAA3F7-B280-41FD-9E33-AA955AC1A934}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
New 6th elves waiting data from mazzo PC
</commit_message>
<xml_diff>
--- a/stats/statistics.xlsx
+++ b/stats/statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b09a39bcc1012fce/Documents/UniPr/magistrale/secondo_semestre/so_e_tempo_reale/programmi_sort/SantaClausProblem/stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{67ED1DCB-23F7-4196-AB18-5D8FACEDEB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{651A0364-A290-47F9-86F2-09157BE6BEC2}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{67ED1DCB-23F7-4196-AB18-5D8FACEDEB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08515505-93B2-4595-916B-6715E4E800B5}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12216" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12216" tabRatio="745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Delivery time" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Elves waiting time (3rd)" sheetId="5" r:id="rId5"/>
     <sheet name="Elves waiting time (4th)" sheetId="6" r:id="rId6"/>
     <sheet name="Elves waiting time (5th)" sheetId="7" r:id="rId7"/>
+    <sheet name="Elves waiting time (6th)" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="25">
   <si>
     <t>santa_v1</t>
   </si>
@@ -287,6 +288,32 @@
   <si>
     <t>ASUS TUF Gaming F15</t>
   </si>
+  <si>
+    <r>
+      <t>Elves waiting time in ms (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>santa_v3, list</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) 6th</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -479,6 +506,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -488,13 +516,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
     <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="43">
     <dxf>
       <font>
         <b val="0"/>
@@ -631,6 +658,133 @@
           <bgColor rgb="FFFF6D6D"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2447,71 +2601,143 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>335279</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>78738</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>144779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Immagine 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AC60D99-9E0D-047F-6413-FFDB2EEDA54D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="24870" t="20139" r="12110" b="11111"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6149339" y="845820"/>
+          <a:ext cx="5839459" cy="4777739"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18B675D9-1A46-4B9E-8A28-DDFCD9E39F51}" name="Tabella1" displayName="Tabella1" ref="B4:F52" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18B675D9-1A46-4B9E-8A28-DDFCD9E39F51}" name="Tabella1" displayName="Tabella1" ref="B4:F52" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="B4:F52" xr:uid="{18B675D9-1A46-4B9E-8A28-DDFCD9E39F51}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{68C9793C-3CE7-40C5-B12A-8900F1F2BC58}" name="#reindeer" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{02981B51-D820-4A61-8F87-5C973297C766}" name="#elves" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{BBBA96F3-B363-4150-A57C-F38AED59221F}" name="#santa" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{6F893902-C0F0-4313-A514-12FA6DFF381E}" name="Avergage" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{86D7F058-3DD3-4FED-B4FF-C7E1D0D0CEED}" name="Std.Dev." dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{68C9793C-3CE7-40C5-B12A-8900F1F2BC58}" name="#reindeer" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{02981B51-D820-4A61-8F87-5C973297C766}" name="#elves" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{BBBA96F3-B363-4150-A57C-F38AED59221F}" name="#santa" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{6F893902-C0F0-4313-A514-12FA6DFF381E}" name="Avergage" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{86D7F058-3DD3-4FED-B4FF-C7E1D0D0CEED}" name="Std.Dev." dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A39B2A33-B243-42A1-B8FE-DC2DD0CC89D6}" name="Tabella13" displayName="Tabella13" ref="B4:F52" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A39B2A33-B243-42A1-B8FE-DC2DD0CC89D6}" name="Tabella13" displayName="Tabella13" ref="B4:F52" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="B4:F52" xr:uid="{A39B2A33-B243-42A1-B8FE-DC2DD0CC89D6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D919451E-F7E6-4920-8AF3-89CB7875E493}" name="#reindeer" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{6173E1FA-D16C-4D56-9D2C-874660ECBECC}" name="#elves" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{69AF351C-DC2C-4E81-B786-EAA98C834955}" name="#santa" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{3D88D429-D733-4965-811A-0B0F4C5261A2}" name="Avergage" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{F1CE163C-D627-41C8-B06D-6834C35A9C2D}" name="Std.Dev." dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{D919451E-F7E6-4920-8AF3-89CB7875E493}" name="#reindeer" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{6173E1FA-D16C-4D56-9D2C-874660ECBECC}" name="#elves" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{69AF351C-DC2C-4E81-B786-EAA98C834955}" name="#santa" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{3D88D429-D733-4965-811A-0B0F4C5261A2}" name="Avergage" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{F1CE163C-D627-41C8-B06D-6834C35A9C2D}" name="Std.Dev." dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D62AA6BD-778C-4B8C-819D-731AAC815ED4}" name="Tabella134" displayName="Tabella134" ref="B4:F52" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D62AA6BD-778C-4B8C-819D-731AAC815ED4}" name="Tabella134" displayName="Tabella134" ref="B4:F52" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="B4:F52" xr:uid="{D62AA6BD-778C-4B8C-819D-731AAC815ED4}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{57B6EDB4-68BC-452C-A1CC-F02DF4D8D251}" name="#reindeer" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{D203EB9D-013C-4F7C-A372-3FB7CB2A5888}" name="#elves" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{52061BDA-34A7-470C-AA2F-8E68C8608C63}" name="#santa" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{3BB9B3CE-8B9C-48BE-B38A-1C73C2521F7E}" name="Avergage" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{BCC6D40D-FE2C-4585-B668-27AEEC8E9FD5}" name="Std.Dev." dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{57B6EDB4-68BC-452C-A1CC-F02DF4D8D251}" name="#reindeer" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{D203EB9D-013C-4F7C-A372-3FB7CB2A5888}" name="#elves" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{52061BDA-34A7-470C-AA2F-8E68C8608C63}" name="#santa" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{3BB9B3CE-8B9C-48BE-B38A-1C73C2521F7E}" name="Avergage" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{BCC6D40D-FE2C-4585-B668-27AEEC8E9FD5}" name="Std.Dev." dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{845B5C2A-09D4-4A3A-B84E-D1FFE2298ED8}" name="Tabella1345" displayName="Tabella1345" ref="B4:F52" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{845B5C2A-09D4-4A3A-B84E-D1FFE2298ED8}" name="Tabella1345" displayName="Tabella1345" ref="B4:F52" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="B4:F52" xr:uid="{845B5C2A-09D4-4A3A-B84E-D1FFE2298ED8}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7B943B3A-9A89-4F9F-A853-5A9814D469E3}" name="#reindeer" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{A6EEF20A-E28C-4A48-8956-795333ACE39D}" name="#elves" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{457D674E-6A2D-4CDE-95DA-23BE2DB06917}" name="#santa" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{75A64399-1220-4A29-BF03-DE8A45A38951}" name="Avergage" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{8BAF1286-C858-4EFA-A585-F7D1D33611FD}" name="Std.Dev." dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{7B943B3A-9A89-4F9F-A853-5A9814D469E3}" name="#reindeer" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{A6EEF20A-E28C-4A48-8956-795333ACE39D}" name="#elves" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{457D674E-6A2D-4CDE-95DA-23BE2DB06917}" name="#santa" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{75A64399-1220-4A29-BF03-DE8A45A38951}" name="Avergage" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{8BAF1286-C858-4EFA-A585-F7D1D33611FD}" name="Std.Dev." dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{20891BED-2C54-4B17-8266-CBD2F440FEE9}" name="Tabella13456" displayName="Tabella13456" ref="B4:F52" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{20891BED-2C54-4B17-8266-CBD2F440FEE9}" name="Tabella13456" displayName="Tabella13456" ref="B4:F52" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="B4:F52" xr:uid="{20891BED-2C54-4B17-8266-CBD2F440FEE9}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9053EC05-B09C-4709-B01A-ACB4CA07722D}" name="#reindeer" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{684A9087-046B-4660-9A40-98D629C59C5F}" name="#elves" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{6E77BF1C-799D-4BE6-B78C-5CA49D1F7BB6}" name="#santa" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{E5670B8F-6E79-4951-A7AA-3021EE6AB1D9}" name="Avergage" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{47117608-6242-4D43-A6C6-C57C9DE4C2B0}" name="Std.Dev." dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9053EC05-B09C-4709-B01A-ACB4CA07722D}" name="#reindeer" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{684A9087-046B-4660-9A40-98D629C59C5F}" name="#elves" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{6E77BF1C-799D-4BE6-B78C-5CA49D1F7BB6}" name="#santa" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{E5670B8F-6E79-4951-A7AA-3021EE6AB1D9}" name="Avergage" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{47117608-6242-4D43-A6C6-C57C9DE4C2B0}" name="Std.Dev." dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{22541FB0-CC03-4CA9-936C-82D047C33671}" name="Tabella134567" displayName="Tabella134567" ref="B4:F52" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="B4:F52" xr:uid="{22541FB0-CC03-4CA9-936C-82D047C33671}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{815672AA-DCAB-4E06-A789-5AE70A21C8D5}" name="#reindeer" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{DFE91DFD-7A26-4677-A6F5-F7D998184E39}" name="#elves" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{DAA0E904-682B-4FA2-9680-DC515022DCD6}" name="#santa" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{5416EB1D-CE31-48C7-BD91-023F0FE2F3EA}" name="Avergage" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{7F2CF403-6CA6-413F-99E3-788BD4DB72E0}" name="Std.Dev." dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2780,11 +3006,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
   <dimension ref="A1:H152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2802,15 +3029,15 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="F3" s="20" t="s">
+      <c r="B3" s="22"/>
+      <c r="F3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="21"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -3978,6 +4205,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5102D166-31D2-4F88-9F57-0DD1511F61E0}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:AE917"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11842,6 +12072,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9318EA9-EF4F-40C4-B40D-C2DECC197DF3}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11865,7 +12098,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -12714,6 +12947,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA8CDDB-7C2F-468C-81CC-A66C991A4AB3}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12737,7 +12973,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -13585,6 +13821,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8722E89F-6CB4-4BA2-B3A4-D0FDFA6617D4}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13608,7 +13847,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -14456,6 +14695,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4BC096-8A3D-4DAD-A146-92F5CE6C6C59}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14479,7 +14721,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -15328,9 +15570,14 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5958168B-79F8-46C8-969C-A8B0B51C678F}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15349,7 +15596,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -16192,6 +16439,880 @@
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD46B91-91AD-467A-907F-2DCA8A4905B1}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:F52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="18"/>
+    <col min="2" max="2" width="14.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="18">
+        <v>9</v>
+      </c>
+      <c r="C5" s="18">
+        <v>3</v>
+      </c>
+      <c r="D5" s="18">
+        <v>1</v>
+      </c>
+      <c r="E5" s="18">
+        <v>25.324762</v>
+      </c>
+      <c r="F5" s="18">
+        <v>212.161372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="18">
+        <v>9</v>
+      </c>
+      <c r="C6" s="18">
+        <v>3</v>
+      </c>
+      <c r="D6" s="18">
+        <v>2</v>
+      </c>
+      <c r="E6" s="18">
+        <v>2.0734620000000001</v>
+      </c>
+      <c r="F6" s="18">
+        <v>16.061627999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="18">
+        <v>9</v>
+      </c>
+      <c r="C7" s="18">
+        <v>4</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1</v>
+      </c>
+      <c r="E7" s="18">
+        <v>30.454374999999999</v>
+      </c>
+      <c r="F7" s="18">
+        <v>247.42264700000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="18">
+        <v>9</v>
+      </c>
+      <c r="C8" s="18">
+        <v>4</v>
+      </c>
+      <c r="D8" s="18">
+        <v>2</v>
+      </c>
+      <c r="E8" s="18">
+        <v>4.952013</v>
+      </c>
+      <c r="F8" s="18">
+        <v>18.022134000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="18">
+        <v>9</v>
+      </c>
+      <c r="C9" s="18">
+        <v>5</v>
+      </c>
+      <c r="D9" s="18">
+        <v>1</v>
+      </c>
+      <c r="E9" s="18">
+        <v>12.467214</v>
+      </c>
+      <c r="F9" s="18">
+        <v>177.047809</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="18">
+        <v>9</v>
+      </c>
+      <c r="C10" s="18">
+        <v>5</v>
+      </c>
+      <c r="D10" s="18">
+        <v>2</v>
+      </c>
+      <c r="E10" s="18">
+        <v>8.0008520000000001</v>
+      </c>
+      <c r="F10" s="18">
+        <v>20.717905999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="18">
+        <v>9</v>
+      </c>
+      <c r="C11" s="18">
+        <v>6</v>
+      </c>
+      <c r="D11" s="18">
+        <v>1</v>
+      </c>
+      <c r="E11" s="18">
+        <v>12.227760999999999</v>
+      </c>
+      <c r="F11" s="18">
+        <v>173.15922599999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="18">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18">
+        <v>6</v>
+      </c>
+      <c r="D12" s="18">
+        <v>2</v>
+      </c>
+      <c r="E12" s="18">
+        <v>11.486280000000001</v>
+      </c>
+      <c r="F12" s="18">
+        <v>24.615341000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="18">
+        <v>9</v>
+      </c>
+      <c r="C13" s="18">
+        <v>6</v>
+      </c>
+      <c r="D13" s="18">
+        <v>3</v>
+      </c>
+      <c r="E13" s="18">
+        <v>1.0440640000000001</v>
+      </c>
+      <c r="F13" s="18">
+        <v>6.8620789999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="18">
+        <v>9</v>
+      </c>
+      <c r="C14" s="18">
+        <v>7</v>
+      </c>
+      <c r="D14" s="18">
+        <v>1</v>
+      </c>
+      <c r="E14" s="18">
+        <v>18.062888000000001</v>
+      </c>
+      <c r="F14" s="18">
+        <v>223.45584500000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="18">
+        <v>9</v>
+      </c>
+      <c r="C15" s="18">
+        <v>7</v>
+      </c>
+      <c r="D15" s="18">
+        <v>2</v>
+      </c>
+      <c r="E15" s="18">
+        <v>14.240508999999999</v>
+      </c>
+      <c r="F15" s="18">
+        <v>25.244962999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="18">
+        <v>9</v>
+      </c>
+      <c r="C16" s="18">
+        <v>7</v>
+      </c>
+      <c r="D16" s="18">
+        <v>3</v>
+      </c>
+      <c r="E16" s="18">
+        <v>2.6232479999999998</v>
+      </c>
+      <c r="F16" s="18">
+        <v>6.0108600000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="18">
+        <v>9</v>
+      </c>
+      <c r="C17" s="18">
+        <v>8</v>
+      </c>
+      <c r="D17" s="18">
+        <v>1</v>
+      </c>
+      <c r="E17" s="18">
+        <v>22.575127999999999</v>
+      </c>
+      <c r="F17" s="18">
+        <v>252.57136800000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="18">
+        <v>9</v>
+      </c>
+      <c r="C18" s="18">
+        <v>8</v>
+      </c>
+      <c r="D18" s="18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="18">
+        <v>17.532720000000001</v>
+      </c>
+      <c r="F18" s="18">
+        <v>27.96876</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="18">
+        <v>9</v>
+      </c>
+      <c r="C19" s="18">
+        <v>8</v>
+      </c>
+      <c r="D19" s="18">
+        <v>3</v>
+      </c>
+      <c r="E19" s="18">
+        <v>4.5417110000000003</v>
+      </c>
+      <c r="F19" s="18">
+        <v>12.104253999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="18">
+        <v>9</v>
+      </c>
+      <c r="C20" s="18">
+        <v>9</v>
+      </c>
+      <c r="D20" s="18">
+        <v>1</v>
+      </c>
+      <c r="E20" s="18">
+        <v>25.598109999999998</v>
+      </c>
+      <c r="F20" s="18">
+        <v>268.209833</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="18">
+        <v>9</v>
+      </c>
+      <c r="C21" s="18">
+        <v>9</v>
+      </c>
+      <c r="D21" s="18">
+        <v>2</v>
+      </c>
+      <c r="E21" s="18">
+        <v>19.758844</v>
+      </c>
+      <c r="F21" s="18">
+        <v>25.579571999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="18">
+        <v>9</v>
+      </c>
+      <c r="C22" s="18">
+        <v>9</v>
+      </c>
+      <c r="D22" s="18">
+        <v>3</v>
+      </c>
+      <c r="E22" s="18">
+        <v>6.1729320000000003</v>
+      </c>
+      <c r="F22" s="18">
+        <v>12.744731</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="18">
+        <v>9</v>
+      </c>
+      <c r="C23" s="18">
+        <v>9</v>
+      </c>
+      <c r="D23" s="18">
+        <v>4</v>
+      </c>
+      <c r="E23" s="18">
+        <v>0.84508499999999998</v>
+      </c>
+      <c r="F23" s="18">
+        <v>7.4958140000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="18">
+        <v>9</v>
+      </c>
+      <c r="C24" s="18">
+        <v>10</v>
+      </c>
+      <c r="D24" s="18">
+        <v>1</v>
+      </c>
+      <c r="E24" s="18">
+        <v>34.469386999999998</v>
+      </c>
+      <c r="F24" s="18">
+        <v>314.89759900000001</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="18">
+        <v>9</v>
+      </c>
+      <c r="C25" s="18">
+        <v>10</v>
+      </c>
+      <c r="D25" s="18">
+        <v>2</v>
+      </c>
+      <c r="E25" s="18">
+        <v>22.504874999999998</v>
+      </c>
+      <c r="F25" s="18">
+        <v>28.920497999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="18">
+        <v>9</v>
+      </c>
+      <c r="C26" s="18">
+        <v>10</v>
+      </c>
+      <c r="D26" s="18">
+        <v>3</v>
+      </c>
+      <c r="E26" s="18">
+        <v>7.57958</v>
+      </c>
+      <c r="F26" s="18">
+        <v>13.111875</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="18">
+        <v>9</v>
+      </c>
+      <c r="C27" s="18">
+        <v>10</v>
+      </c>
+      <c r="D27" s="18">
+        <v>4</v>
+      </c>
+      <c r="E27" s="18">
+        <v>1.881785</v>
+      </c>
+      <c r="F27" s="18">
+        <v>5.2134090000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="18">
+        <v>9</v>
+      </c>
+      <c r="C28" s="18">
+        <v>11</v>
+      </c>
+      <c r="D28" s="18">
+        <v>1</v>
+      </c>
+      <c r="E28" s="18">
+        <v>39.915716000000003</v>
+      </c>
+      <c r="F28" s="18">
+        <v>342.77420100000001</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="18">
+        <v>9</v>
+      </c>
+      <c r="C29" s="18">
+        <v>11</v>
+      </c>
+      <c r="D29" s="18">
+        <v>2</v>
+      </c>
+      <c r="E29" s="18">
+        <v>26.373470000000001</v>
+      </c>
+      <c r="F29" s="18">
+        <v>33.422058999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="18">
+        <v>9</v>
+      </c>
+      <c r="C30" s="18">
+        <v>11</v>
+      </c>
+      <c r="D30" s="18">
+        <v>3</v>
+      </c>
+      <c r="E30" s="18">
+        <v>9.6611049999999992</v>
+      </c>
+      <c r="F30" s="18">
+        <v>14.8918</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="18">
+        <v>9</v>
+      </c>
+      <c r="C31" s="18">
+        <v>11</v>
+      </c>
+      <c r="D31" s="18">
+        <v>4</v>
+      </c>
+      <c r="E31" s="18">
+        <v>3.0745990000000001</v>
+      </c>
+      <c r="F31" s="18">
+        <v>5.8559400000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="18">
+        <v>9</v>
+      </c>
+      <c r="C32" s="18">
+        <v>12</v>
+      </c>
+      <c r="D32" s="18">
+        <v>1</v>
+      </c>
+      <c r="E32" s="18">
+        <v>12.081649000000001</v>
+      </c>
+      <c r="F32" s="18">
+        <v>182.18619000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="18">
+        <v>9</v>
+      </c>
+      <c r="C33" s="18">
+        <v>12</v>
+      </c>
+      <c r="D33" s="18">
+        <v>2</v>
+      </c>
+      <c r="E33" s="18">
+        <v>28.794315000000001</v>
+      </c>
+      <c r="F33" s="18">
+        <v>32.354609000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="18">
+        <v>9</v>
+      </c>
+      <c r="C34" s="18">
+        <v>12</v>
+      </c>
+      <c r="D34" s="18">
+        <v>3</v>
+      </c>
+      <c r="E34" s="18">
+        <v>11.288992</v>
+      </c>
+      <c r="F34" s="18">
+        <v>16.526762999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="18">
+        <v>9</v>
+      </c>
+      <c r="C35" s="18">
+        <v>12</v>
+      </c>
+      <c r="D35" s="18">
+        <v>4</v>
+      </c>
+      <c r="E35" s="18">
+        <v>4.2592030000000003</v>
+      </c>
+      <c r="F35" s="18">
+        <v>8.4612119999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="18">
+        <v>9</v>
+      </c>
+      <c r="C36" s="18">
+        <v>12</v>
+      </c>
+      <c r="D36" s="18">
+        <v>5</v>
+      </c>
+      <c r="E36" s="18">
+        <v>0.84629299999999996</v>
+      </c>
+      <c r="F36" s="18">
+        <v>9.7336200000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="18">
+        <v>9</v>
+      </c>
+      <c r="C37" s="18">
+        <v>13</v>
+      </c>
+      <c r="D37" s="18">
+        <v>1</v>
+      </c>
+      <c r="E37" s="18">
+        <v>11.206227999999999</v>
+      </c>
+      <c r="F37" s="18">
+        <v>170.45582200000001</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="18">
+        <v>9</v>
+      </c>
+      <c r="C38" s="18">
+        <v>13</v>
+      </c>
+      <c r="D38" s="18">
+        <v>2</v>
+      </c>
+      <c r="E38" s="18">
+        <v>32.755223000000001</v>
+      </c>
+      <c r="F38" s="18">
+        <v>38.920794999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="18">
+        <v>9</v>
+      </c>
+      <c r="C39" s="18">
+        <v>13</v>
+      </c>
+      <c r="D39" s="18">
+        <v>3</v>
+      </c>
+      <c r="E39" s="18">
+        <v>12.845834</v>
+      </c>
+      <c r="F39" s="18">
+        <v>15.013631999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="18">
+        <v>9</v>
+      </c>
+      <c r="C40" s="18">
+        <v>13</v>
+      </c>
+      <c r="D40" s="18">
+        <v>4</v>
+      </c>
+      <c r="E40" s="18">
+        <v>5.5195610000000004</v>
+      </c>
+      <c r="F40" s="18">
+        <v>12.651956999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="18">
+        <v>9</v>
+      </c>
+      <c r="C41" s="18">
+        <v>13</v>
+      </c>
+      <c r="D41" s="18">
+        <v>5</v>
+      </c>
+      <c r="E41" s="18">
+        <v>1.5153890000000001</v>
+      </c>
+      <c r="F41" s="18">
+        <v>4.2578930000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="18">
+        <v>9</v>
+      </c>
+      <c r="C42" s="18">
+        <v>14</v>
+      </c>
+      <c r="D42" s="18">
+        <v>1</v>
+      </c>
+      <c r="E42" s="18">
+        <v>11.042353</v>
+      </c>
+      <c r="F42" s="18">
+        <v>169.69864000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="18">
+        <v>9</v>
+      </c>
+      <c r="C43" s="18">
+        <v>14</v>
+      </c>
+      <c r="D43" s="18">
+        <v>2</v>
+      </c>
+      <c r="E43" s="18">
+        <v>35.456325</v>
+      </c>
+      <c r="F43" s="18">
+        <v>40.229112999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="18">
+        <v>9</v>
+      </c>
+      <c r="C44" s="18">
+        <v>14</v>
+      </c>
+      <c r="D44" s="18">
+        <v>3</v>
+      </c>
+      <c r="E44" s="18">
+        <v>14.521820999999999</v>
+      </c>
+      <c r="F44" s="18">
+        <v>15.626598</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="18">
+        <v>9</v>
+      </c>
+      <c r="C45" s="18">
+        <v>14</v>
+      </c>
+      <c r="D45" s="18">
+        <v>4</v>
+      </c>
+      <c r="E45" s="18">
+        <v>6.5677130000000004</v>
+      </c>
+      <c r="F45" s="18">
+        <v>10.536246999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="18">
+        <v>9</v>
+      </c>
+      <c r="C46" s="18">
+        <v>14</v>
+      </c>
+      <c r="D46" s="18">
+        <v>5</v>
+      </c>
+      <c r="E46" s="18">
+        <v>2.442059</v>
+      </c>
+      <c r="F46" s="18">
+        <v>6.1958000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="18">
+        <v>9</v>
+      </c>
+      <c r="C47" s="18">
+        <v>15</v>
+      </c>
+      <c r="D47" s="18">
+        <v>1</v>
+      </c>
+      <c r="E47" s="18">
+        <v>11.123818999999999</v>
+      </c>
+      <c r="F47" s="18">
+        <v>169.315168</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="18">
+        <v>9</v>
+      </c>
+      <c r="C48" s="18">
+        <v>15</v>
+      </c>
+      <c r="D48" s="18">
+        <v>2</v>
+      </c>
+      <c r="E48" s="18">
+        <v>38.256996999999998</v>
+      </c>
+      <c r="F48" s="18">
+        <v>39.933827000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="18">
+        <v>9</v>
+      </c>
+      <c r="C49" s="18">
+        <v>15</v>
+      </c>
+      <c r="D49" s="18">
+        <v>3</v>
+      </c>
+      <c r="E49" s="18">
+        <v>16.300968999999998</v>
+      </c>
+      <c r="F49" s="18">
+        <v>17.772068000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="18">
+        <v>9</v>
+      </c>
+      <c r="C50" s="18">
+        <v>15</v>
+      </c>
+      <c r="D50" s="18">
+        <v>4</v>
+      </c>
+      <c r="E50" s="18">
+        <v>7.8499939999999997</v>
+      </c>
+      <c r="F50" s="18">
+        <v>11.850743</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="18">
+        <v>9</v>
+      </c>
+      <c r="C51" s="18">
+        <v>15</v>
+      </c>
+      <c r="D51" s="18">
+        <v>5</v>
+      </c>
+      <c r="E51" s="18">
+        <v>3.4269379999999998</v>
+      </c>
+      <c r="F51" s="18">
+        <v>8.4907280000000007</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="18">
+        <v>9</v>
+      </c>
+      <c r="C52" s="18">
+        <v>15</v>
+      </c>
+      <c r="D52" s="18">
+        <v>6</v>
+      </c>
+      <c r="E52" s="18">
+        <v>0.73825600000000002</v>
+      </c>
+      <c r="F52" s="18">
+        <v>5.2123200000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>